<commit_message>
pak tri habis hapus kak novisa
</commit_message>
<xml_diff>
--- a/database/data_notel_dari_rizal/endah.xlsx
+++ b/database/data_notel_dari_rizal/endah.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ucup_d\yabuki\database\data_notel_dari_rizal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5F0E3B-FDCE-4B4F-8007-872E30D43B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF862347-8098-41F3-86F9-AFE0C253D5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="3195" windowWidth="12660" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
   <dimension ref="A1:E300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
pa tri input database baru klasifikasi per dn
</commit_message>
<xml_diff>
--- a/database/data_notel_dari_rizal/endah.xlsx
+++ b/database/data_notel_dari_rizal/endah.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ucup_d\yabuki\database\data_notel_dari_rizal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF862347-8098-41F3-86F9-AFE0C253D5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4A5D9E-84B9-44E1-945C-54E7148E6D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="12660" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -30,309 +30,159 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
-  <si>
-    <t>62811262661</t>
-  </si>
-  <si>
-    <t>62811262662</t>
-  </si>
-  <si>
-    <t>62811262663</t>
-  </si>
-  <si>
-    <t>62811262664</t>
-  </si>
-  <si>
-    <t>62811262665</t>
-  </si>
-  <si>
-    <t>62811262666</t>
-  </si>
-  <si>
-    <t>62811262669</t>
-  </si>
-  <si>
-    <t>62811262671</t>
-  </si>
-  <si>
-    <t>62811262673</t>
-  </si>
-  <si>
-    <t>62811262674</t>
-  </si>
-  <si>
-    <t>62811262676</t>
-  </si>
-  <si>
-    <t>62811262677</t>
-  </si>
-  <si>
-    <t>62811262678</t>
-  </si>
-  <si>
-    <t>62811262679</t>
-  </si>
-  <si>
-    <t>62811262680</t>
-  </si>
-  <si>
-    <t>62811262681</t>
-  </si>
-  <si>
-    <t>62811262683</t>
-  </si>
-  <si>
-    <t>62811262688</t>
-  </si>
-  <si>
-    <t>62811262689</t>
-  </si>
-  <si>
-    <t>62811262691</t>
-  </si>
-  <si>
-    <t>62811262693</t>
-  </si>
-  <si>
-    <t>62811262694</t>
-  </si>
-  <si>
-    <t>62811262695</t>
-  </si>
-  <si>
-    <t>62811262696</t>
-  </si>
-  <si>
-    <t>62811262699</t>
-  </si>
-  <si>
-    <t>62811262700</t>
-  </si>
-  <si>
-    <t>62811262707</t>
-  </si>
-  <si>
-    <t>62811262711</t>
-  </si>
-  <si>
-    <t>62811262712</t>
-  </si>
-  <si>
-    <t>62811262718</t>
-  </si>
-  <si>
-    <t>62811262721</t>
-  </si>
-  <si>
-    <t>62811262722</t>
-  </si>
-  <si>
-    <t>62811262726</t>
-  </si>
-  <si>
-    <t>62811262727</t>
-  </si>
-  <si>
-    <t>62811262728</t>
-  </si>
-  <si>
-    <t>62811262729</t>
-  </si>
-  <si>
-    <t>62811262730</t>
-  </si>
-  <si>
-    <t>62811262740</t>
-  </si>
-  <si>
-    <t>62811262747</t>
-  </si>
-  <si>
-    <t>62811262750</t>
-  </si>
-  <si>
-    <t>62811262755</t>
-  </si>
-  <si>
-    <t>62811262758</t>
-  </si>
-  <si>
-    <t>62811262766</t>
-  </si>
-  <si>
-    <t>62811262767</t>
-  </si>
-  <si>
-    <t>62811262769</t>
-  </si>
-  <si>
-    <t>62811262770</t>
-  </si>
-  <si>
-    <t>62811262771</t>
-  </si>
-  <si>
-    <t>62811262772</t>
-  </si>
-  <si>
-    <t>62811262775</t>
-  </si>
-  <si>
-    <t>62811262776</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>no_telpon</t>
   </si>
   <si>
-    <t>62811263433</t>
-  </si>
-  <si>
-    <t>62811263434</t>
-  </si>
-  <si>
-    <t>62811263437</t>
-  </si>
-  <si>
-    <t>62811263440</t>
-  </si>
-  <si>
-    <t>62811263442</t>
-  </si>
-  <si>
-    <t>62811263443</t>
-  </si>
-  <si>
-    <t>62811263444</t>
-  </si>
-  <si>
-    <t>62811263446</t>
-  </si>
-  <si>
-    <t>62811263447</t>
-  </si>
-  <si>
-    <t>62811263449</t>
-  </si>
-  <si>
-    <t>62811263453</t>
-  </si>
-  <si>
-    <t>62811263454</t>
-  </si>
-  <si>
-    <t>62811263455</t>
-  </si>
-  <si>
-    <t>62811263460</t>
-  </si>
-  <si>
-    <t>62811263461</t>
-  </si>
-  <si>
-    <t>62811263463</t>
-  </si>
-  <si>
-    <t>62811263466</t>
-  </si>
-  <si>
-    <t>62811263467</t>
-  </si>
-  <si>
-    <t>62811263468</t>
-  </si>
-  <si>
-    <t>62811263470</t>
-  </si>
-  <si>
-    <t>62811263477</t>
-  </si>
-  <si>
-    <t>62811263483</t>
-  </si>
-  <si>
-    <t>62811263484</t>
-  </si>
-  <si>
-    <t>62811263488</t>
-  </si>
-  <si>
-    <t>62811263495</t>
-  </si>
-  <si>
-    <t>62811263506</t>
-  </si>
-  <si>
-    <t>62811263513</t>
-  </si>
-  <si>
-    <t>62811263515</t>
-  </si>
-  <si>
-    <t>62811263516</t>
-  </si>
-  <si>
-    <t>62811263517</t>
-  </si>
-  <si>
-    <t>62811263520</t>
-  </si>
-  <si>
-    <t>62811263521</t>
-  </si>
-  <si>
-    <t>62811263522</t>
-  </si>
-  <si>
-    <t>62811263525</t>
-  </si>
-  <si>
-    <t>62811263533</t>
-  </si>
-  <si>
-    <t>62811263535</t>
-  </si>
-  <si>
-    <t>62811263536</t>
-  </si>
-  <si>
-    <t>62811263537</t>
-  </si>
-  <si>
-    <t>62811263543</t>
-  </si>
-  <si>
-    <t>62811263545</t>
-  </si>
-  <si>
-    <t>62811263549</t>
-  </si>
-  <si>
-    <t>62811263550</t>
-  </si>
-  <si>
-    <t>62811263551</t>
-  </si>
-  <si>
-    <t>62811263553</t>
-  </si>
-  <si>
-    <t>62811263555</t>
-  </si>
-  <si>
-    <t>62811263557</t>
-  </si>
-  <si>
-    <t>62811263558</t>
-  </si>
-  <si>
-    <t>62811263559</t>
-  </si>
-  <si>
-    <t>62811263562</t>
-  </si>
-  <si>
-    <t>62811263563</t>
+    <t>62811264687</t>
+  </si>
+  <si>
+    <t>62811264688</t>
+  </si>
+  <si>
+    <t>62811264692</t>
+  </si>
+  <si>
+    <t>62811264696</t>
+  </si>
+  <si>
+    <t>62811264699</t>
+  </si>
+  <si>
+    <t>62811264700</t>
+  </si>
+  <si>
+    <t>62811264704</t>
+  </si>
+  <si>
+    <t>62811264708</t>
+  </si>
+  <si>
+    <t>62811264709</t>
+  </si>
+  <si>
+    <t>62811264712</t>
+  </si>
+  <si>
+    <t>62811264717</t>
+  </si>
+  <si>
+    <t>62811264718</t>
+  </si>
+  <si>
+    <t>62811264719</t>
+  </si>
+  <si>
+    <t>62811264723</t>
+  </si>
+  <si>
+    <t>62811264725</t>
+  </si>
+  <si>
+    <t>62811264733</t>
+  </si>
+  <si>
+    <t>62811264735</t>
+  </si>
+  <si>
+    <t>62811264738</t>
+  </si>
+  <si>
+    <t>62811264741</t>
+  </si>
+  <si>
+    <t>62811264742</t>
+  </si>
+  <si>
+    <t>62811264747</t>
+  </si>
+  <si>
+    <t>62811264748</t>
+  </si>
+  <si>
+    <t>62811264750</t>
+  </si>
+  <si>
+    <t>62811264752</t>
+  </si>
+  <si>
+    <t>62811264755</t>
+  </si>
+  <si>
+    <t>62811264756</t>
+  </si>
+  <si>
+    <t>62811264757</t>
+  </si>
+  <si>
+    <t>62811264759</t>
+  </si>
+  <si>
+    <t>62811264764</t>
+  </si>
+  <si>
+    <t>62811264768</t>
+  </si>
+  <si>
+    <t>62811264772</t>
+  </si>
+  <si>
+    <t>62811264774</t>
+  </si>
+  <si>
+    <t>62811264775</t>
+  </si>
+  <si>
+    <t>62811264784</t>
+  </si>
+  <si>
+    <t>62811264786</t>
+  </si>
+  <si>
+    <t>62811264788</t>
+  </si>
+  <si>
+    <t>62811264789</t>
+  </si>
+  <si>
+    <t>62811264795</t>
+  </si>
+  <si>
+    <t>62811264797</t>
+  </si>
+  <si>
+    <t>62811264800</t>
+  </si>
+  <si>
+    <t>62811264804</t>
+  </si>
+  <si>
+    <t>62811264811</t>
+  </si>
+  <si>
+    <t>62811264813</t>
+  </si>
+  <si>
+    <t>62811264815</t>
+  </si>
+  <si>
+    <t>62811264818</t>
+  </si>
+  <si>
+    <t>62811264820</t>
+  </si>
+  <si>
+    <t>62811264822</t>
+  </si>
+  <si>
+    <t>62811264825</t>
+  </si>
+  <si>
+    <t>62811264826</t>
+  </si>
+  <si>
+    <t>62811264828</t>
   </si>
 </sst>
 </file>
@@ -384,13 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2827B066-A96F-1349-9FFA-95B9370F4143}">
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,506 +577,356 @@
       <c r="A1" s="2"/>
       <c r="B1" s="1"/>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>51</v>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>53</v>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>54</v>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>55</v>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>56</v>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>57</v>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>58</v>
+      <c r="E9" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>59</v>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>60</v>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>61</v>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>62</v>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>63</v>
+      <c r="E14" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>64</v>
+      <c r="E15" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>65</v>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>66</v>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>67</v>
+      <c r="E18" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>68</v>
+      <c r="E19" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>69</v>
+      <c r="E20" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>70</v>
+      <c r="E21" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>71</v>
+      <c r="E22" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>72</v>
+      <c r="E23" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>73</v>
+      <c r="E24" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>74</v>
+      <c r="E25" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>75</v>
+      <c r="E26" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>76</v>
+      <c r="E27" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>77</v>
+      <c r="E28" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>78</v>
+      <c r="E29" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>79</v>
+      <c r="E30" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>80</v>
+      <c r="E31" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>81</v>
+      <c r="E32" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>82</v>
+      <c r="E33" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>83</v>
+      <c r="E34" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>84</v>
+      <c r="E35" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>85</v>
+      <c r="E36" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>86</v>
+      <c r="E37" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>87</v>
+      <c r="E38" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>88</v>
+      <c r="E39" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>89</v>
+      <c r="E40" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>90</v>
+      <c r="E41" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>91</v>
+      <c r="E42" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" t="s">
-        <v>41</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>92</v>
+      <c r="E43" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>93</v>
+      <c r="E44" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>94</v>
+      <c r="E45" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>95</v>
+      <c r="E46" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" t="s">
-        <v>45</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>96</v>
+      <c r="E47" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" t="s">
-        <v>46</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>97</v>
+      <c r="E48" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" t="s">
-        <v>47</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>98</v>
+      <c r="E49" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" t="s">
-        <v>48</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>99</v>
+      <c r="E50" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="C51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>100</v>
+      <c r="E51" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>